<commit_message>
wip buy 0 house problem
</commit_message>
<xml_diff>
--- a/LifeCycleData.xlsx
+++ b/LifeCycleData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Christian/Dropbox/KU - Polit/KA/Thesis/MScThesis-2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5302D3C1-04F4-1A43-B1B5-58D0D9D4E293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABBD7F6-4239-2B44-9F0D-39CE968D5604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13420" tabRatio="676" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13420" tabRatio="676" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HoOutput" sheetId="10" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="595">
   <si>
     <t>Forbrug efter prisenhed, forbrugsgruppe, alder og tid</t>
   </si>
@@ -1820,6 +1820,12 @@
   </si>
   <si>
     <t>Ownershare</t>
+  </si>
+  <si>
+    <t>normalised net wealth</t>
+  </si>
+  <si>
+    <t>percentiles</t>
   </si>
 </sst>
 </file>
@@ -1985,6 +1991,1175 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="nb-NO"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nb-NO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Net_wealth_compute!$O$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>normalised net wealth</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Net_wealth_compute!$N$4:$N$110</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Net_wealth_compute!$O$4:$O$110</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>7.1641791044776124E-2</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.2582089552238806</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.72835820895522385</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1.1686567164179105</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2.4925373134328357</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E9F7-BE42-974E-CAF1FA40675C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="867040367"/>
+        <c:axId val="866528607"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="867040367"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nb-NO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="866528607"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="866528607"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nb-NO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="867040367"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nb-NO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -2033,6 +3208,42 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>273050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagram 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB2AA599-81AB-3940-9AFC-7F470A417742}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2325,7 +3536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEDA33B8-DBDA-674D-9995-E7671E40D99A}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -4587,10 +5798,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66045958-6ECB-4C23-8917-618C98274AD9}">
-  <dimension ref="A1:M76"/>
+  <dimension ref="A1:O110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4604,9 +5815,11 @@
     <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.33203125" customWidth="1"/>
     <col min="13" max="13" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" customWidth="1"/>
+    <col min="15" max="15" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16">
+    <row r="1" spans="1:15" ht="16">
       <c r="A1" s="16" t="s">
         <v>21</v>
       </c>
@@ -4614,10 +5827,10 @@
         <v>569</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:15">
       <c r="A2" s="9"/>
     </row>
-    <row r="3" spans="1:13" ht="17">
+    <row r="3" spans="1:15" ht="19" customHeight="1">
       <c r="A3" s="10" t="s">
         <v>22</v>
       </c>
@@ -4651,8 +5864,14 @@
       <c r="K3" s="10" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="17" hidden="1">
+      <c r="N3" s="10" t="s">
+        <v>594</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="17" hidden="1">
       <c r="A4" s="11">
         <v>18</v>
       </c>
@@ -4686,7 +5905,7 @@
       </c>
       <c r="M4" s="8"/>
     </row>
-    <row r="5" spans="1:13" ht="17" hidden="1">
+    <row r="5" spans="1:15" ht="17" hidden="1">
       <c r="A5" s="13">
         <v>19</v>
       </c>
@@ -4719,7 +5938,7 @@
         <v>71000</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="17" hidden="1">
+    <row r="6" spans="1:15" ht="17" hidden="1">
       <c r="A6" s="11">
         <v>20</v>
       </c>
@@ -4752,7 +5971,7 @@
         <v>83000</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="17" hidden="1">
+    <row r="7" spans="1:15" ht="17" hidden="1">
       <c r="A7" s="13">
         <v>21</v>
       </c>
@@ -4785,7 +6004,7 @@
         <v>110000</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="17" hidden="1">
+    <row r="8" spans="1:15" ht="17" hidden="1">
       <c r="A8" s="11">
         <v>22</v>
       </c>
@@ -4818,7 +6037,7 @@
         <v>120000</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="17" hidden="1">
+    <row r="9" spans="1:15" ht="17" hidden="1">
       <c r="A9" s="13">
         <v>23</v>
       </c>
@@ -4851,7 +6070,7 @@
         <v>126000</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="17" hidden="1">
+    <row r="10" spans="1:15" ht="17" hidden="1">
       <c r="A10" s="11">
         <v>24</v>
       </c>
@@ -4884,7 +6103,7 @@
         <v>136000</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="17">
+    <row r="11" spans="1:15" ht="17">
       <c r="A11" s="13">
         <v>25</v>
       </c>
@@ -4920,8 +6139,14 @@
         <f>J11/670000</f>
         <v>0.24328358208955222</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="17">
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="17">
       <c r="A12" s="11">
         <v>26</v>
       </c>
@@ -4957,8 +6182,11 @@
         <f t="shared" ref="K12:K66" si="2">J12/670000</f>
         <v>0.29701492537313434</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="17">
+      <c r="N12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="17">
       <c r="A13" s="13">
         <v>27</v>
       </c>
@@ -4994,8 +6222,11 @@
         <f t="shared" si="2"/>
         <v>0.3</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="17">
+      <c r="N13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="17">
       <c r="A14" s="11">
         <v>28</v>
       </c>
@@ -5031,8 +6262,11 @@
         <f t="shared" si="2"/>
         <v>0.34328358208955223</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="17">
+      <c r="N14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="17">
       <c r="A15" s="13">
         <v>29</v>
       </c>
@@ -5068,8 +6302,11 @@
         <f t="shared" si="2"/>
         <v>0.37761194029850748</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="17">
+      <c r="N15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="17">
       <c r="A16" s="11">
         <v>30</v>
       </c>
@@ -5105,8 +6342,11 @@
         <f t="shared" si="2"/>
         <v>0.45522388059701491</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="17">
+      <c r="N16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="17">
       <c r="A17" s="13">
         <v>31</v>
       </c>
@@ -5142,8 +6382,11 @@
         <f t="shared" si="2"/>
         <v>0.5164179104477612</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="17">
+      <c r="N17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="17">
       <c r="A18" s="11">
         <v>32</v>
       </c>
@@ -5179,8 +6422,11 @@
         <f t="shared" si="2"/>
         <v>0.61791044776119408</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="17">
+      <c r="N18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="17">
       <c r="A19" s="13">
         <v>33</v>
       </c>
@@ -5216,8 +6462,11 @@
         <f t="shared" si="2"/>
         <v>0.64029850746268657</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="17">
+      <c r="N19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="17">
       <c r="A20" s="11">
         <v>34</v>
       </c>
@@ -5253,8 +6502,11 @@
         <f t="shared" si="2"/>
         <v>0.72238805970149256</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="17">
+      <c r="N20">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="17">
       <c r="A21" s="13">
         <v>35</v>
       </c>
@@ -5290,8 +6542,11 @@
         <f t="shared" si="2"/>
         <v>0.80149253731343284</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="17">
+      <c r="N21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="17">
       <c r="A22" s="11">
         <v>36</v>
       </c>
@@ -5327,8 +6582,11 @@
         <f t="shared" si="2"/>
         <v>0.87462686567164183</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="17">
+      <c r="N22">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="17">
       <c r="A23" s="13">
         <v>37</v>
       </c>
@@ -5364,8 +6622,11 @@
         <f t="shared" si="2"/>
         <v>0.9761194029850746</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="17">
+      <c r="N23">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="17">
       <c r="A24" s="11">
         <v>38</v>
       </c>
@@ -5401,8 +6662,11 @@
         <f t="shared" si="2"/>
         <v>1.0537313432835822</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="17">
+      <c r="N24">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="17">
       <c r="A25" s="13">
         <v>39</v>
       </c>
@@ -5438,8 +6702,11 @@
         <f t="shared" si="2"/>
         <v>1.1776119402985075</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="17">
+      <c r="N25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="17">
       <c r="A26" s="11">
         <v>40</v>
       </c>
@@ -5475,8 +6742,11 @@
         <f t="shared" si="2"/>
         <v>1.2686567164179106</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" ht="17">
+      <c r="N26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="17">
       <c r="A27" s="13">
         <v>41</v>
       </c>
@@ -5512,8 +6782,11 @@
         <f t="shared" si="2"/>
         <v>1.3820895522388059</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="17">
+      <c r="N27">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="17">
       <c r="A28" s="11">
         <v>42</v>
       </c>
@@ -5549,8 +6822,11 @@
         <f t="shared" si="2"/>
         <v>1.4895522388059701</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" ht="17">
+      <c r="N28">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="17">
       <c r="A29" s="13">
         <v>43</v>
       </c>
@@ -5586,8 +6862,11 @@
         <f t="shared" si="2"/>
         <v>1.5626865671641792</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="17">
+      <c r="N29">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="17">
       <c r="A30" s="11">
         <v>44</v>
       </c>
@@ -5623,8 +6902,11 @@
         <f t="shared" si="2"/>
         <v>1.7208955223880598</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" ht="17">
+      <c r="N30">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="17">
       <c r="A31" s="13">
         <v>45</v>
       </c>
@@ -5660,8 +6942,11 @@
         <f t="shared" si="2"/>
         <v>1.8313432835820895</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" ht="17">
+      <c r="N31">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="17">
       <c r="A32" s="11">
         <v>46</v>
       </c>
@@ -5697,8 +6982,11 @@
         <f t="shared" si="2"/>
         <v>1.9194029850746268</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" ht="17">
+      <c r="N32">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="17">
       <c r="A33" s="13">
         <v>47</v>
       </c>
@@ -5734,8 +7022,11 @@
         <f t="shared" si="2"/>
         <v>2.0014925373134327</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" ht="17">
+      <c r="N33">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="17">
       <c r="A34" s="11">
         <v>48</v>
       </c>
@@ -5771,8 +7062,11 @@
         <f t="shared" si="2"/>
         <v>2.0880597014925373</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" ht="17">
+      <c r="N34">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="17">
       <c r="A35" s="13">
         <v>49</v>
       </c>
@@ -5808,8 +7102,11 @@
         <f t="shared" si="2"/>
         <v>2.1686567164179102</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" ht="17">
+      <c r="N35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="17">
       <c r="A36" s="11">
         <v>50</v>
       </c>
@@ -5845,8 +7142,14 @@
         <f t="shared" si="2"/>
         <v>2.2895522388059701</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" ht="17">
+      <c r="N36">
+        <v>25</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="17">
       <c r="A37" s="13">
         <v>51</v>
       </c>
@@ -5882,8 +7185,11 @@
         <f t="shared" si="2"/>
         <v>2.4134328358208954</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" ht="17">
+      <c r="N37">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="17">
       <c r="A38" s="11">
         <v>52</v>
       </c>
@@ -5919,8 +7225,11 @@
         <f t="shared" si="2"/>
         <v>2.5029850746268658</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" ht="17">
+      <c r="N38">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="17">
       <c r="A39" s="13">
         <v>53</v>
       </c>
@@ -5956,8 +7265,11 @@
         <f t="shared" si="2"/>
         <v>2.6447761194029851</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" ht="17">
+      <c r="N39">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="17">
       <c r="A40" s="11">
         <v>54</v>
       </c>
@@ -5993,8 +7305,11 @@
         <f t="shared" si="2"/>
         <v>2.6910447761194032</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" ht="17">
+      <c r="N40">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="17">
       <c r="A41" s="13">
         <v>55</v>
       </c>
@@ -6030,8 +7345,11 @@
         <f t="shared" si="2"/>
         <v>2.8805970149253732</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" ht="17">
+      <c r="N41">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="17">
       <c r="A42" s="11">
         <v>56</v>
       </c>
@@ -6067,8 +7385,11 @@
         <f t="shared" si="2"/>
         <v>2.9776119402985075</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" ht="17">
+      <c r="N42">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="17">
       <c r="A43" s="13">
         <v>57</v>
       </c>
@@ -6104,8 +7425,11 @@
         <f t="shared" si="2"/>
         <v>3.1955223880597017</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" ht="17">
+      <c r="N43">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="17">
       <c r="A44" s="11">
         <v>58</v>
       </c>
@@ -6141,8 +7465,11 @@
         <f t="shared" si="2"/>
         <v>3.2179104477611942</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" ht="17">
+      <c r="N44">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="17">
       <c r="A45" s="13">
         <v>59</v>
       </c>
@@ -6178,8 +7505,11 @@
         <f t="shared" si="2"/>
         <v>3.3671641791044777</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" ht="17">
+      <c r="N45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="17">
       <c r="A46" s="11">
         <v>60</v>
       </c>
@@ -6215,8 +7545,11 @@
         <f t="shared" si="2"/>
         <v>3.5582089552238805</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" ht="17">
+      <c r="N46">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="17">
       <c r="A47" s="13">
         <v>61</v>
       </c>
@@ -6252,8 +7585,11 @@
         <f t="shared" si="2"/>
         <v>3.5880597014925373</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" ht="17">
+      <c r="N47">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="17">
       <c r="A48" s="11">
         <v>62</v>
       </c>
@@ -6289,8 +7625,11 @@
         <f t="shared" si="2"/>
         <v>3.7089552238805972</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" ht="17">
+      <c r="N48">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="17">
       <c r="A49" s="13">
         <v>63</v>
       </c>
@@ -6326,8 +7665,11 @@
         <f t="shared" si="2"/>
         <v>3.8283582089552239</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" ht="17">
+      <c r="N49">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="17">
       <c r="A50" s="11">
         <v>64</v>
       </c>
@@ -6363,8 +7705,11 @@
         <f t="shared" si="2"/>
         <v>3.9208955223880597</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" ht="17">
+      <c r="N50">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="17">
       <c r="A51" s="13">
         <v>65</v>
       </c>
@@ -6400,8 +7745,11 @@
         <f t="shared" si="2"/>
         <v>3.8522388059701491</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" ht="17">
+      <c r="N51">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" ht="17">
       <c r="A52" s="11">
         <v>66</v>
       </c>
@@ -6437,8 +7785,11 @@
         <f t="shared" si="2"/>
         <v>3.9238805970149255</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" ht="17">
+      <c r="N52">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="17">
       <c r="A53" s="13">
         <v>67</v>
       </c>
@@ -6474,8 +7825,11 @@
         <f t="shared" si="2"/>
         <v>3.946268656716418</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" ht="17">
+      <c r="N53">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="17">
       <c r="A54" s="11">
         <v>68</v>
       </c>
@@ -6511,8 +7865,11 @@
         <f t="shared" si="2"/>
         <v>3.7970149253731345</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" ht="17">
+      <c r="N54">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="17">
       <c r="A55" s="13">
         <v>69</v>
       </c>
@@ -6548,8 +7905,11 @@
         <f t="shared" si="2"/>
         <v>3.8059701492537314</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" ht="17">
+      <c r="N55">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="17">
       <c r="A56" s="11">
         <v>70</v>
       </c>
@@ -6585,8 +7945,11 @@
         <f t="shared" si="2"/>
         <v>3.8268656716417913</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" ht="17">
+      <c r="N56">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="17">
       <c r="A57" s="13">
         <v>71</v>
       </c>
@@ -6622,8 +7985,11 @@
         <f t="shared" si="2"/>
         <v>3.9776119402985075</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" ht="17">
+      <c r="N57">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="17">
       <c r="A58" s="11">
         <v>72</v>
       </c>
@@ -6659,8 +8025,11 @@
         <f t="shared" si="2"/>
         <v>3.6582089552238806</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" ht="17">
+      <c r="N58">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" ht="17">
       <c r="A59" s="13">
         <v>73</v>
       </c>
@@ -6696,8 +8065,11 @@
         <f t="shared" si="2"/>
         <v>3.783582089552239</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" ht="17">
+      <c r="N59">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" ht="17">
       <c r="A60" s="11">
         <v>74</v>
       </c>
@@ -6733,8 +8105,11 @@
         <f t="shared" si="2"/>
         <v>3.4313432835820894</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" ht="17">
+      <c r="N60">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" ht="17">
       <c r="A61" s="13">
         <v>75</v>
       </c>
@@ -6770,8 +8145,15 @@
         <f t="shared" si="2"/>
         <v>3.4223880597014924</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" ht="17">
+      <c r="N61">
+        <v>50</v>
+      </c>
+      <c r="O61">
+        <f>48000/670000</f>
+        <v>7.1641791044776124E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" ht="17">
       <c r="A62" s="11">
         <v>76</v>
       </c>
@@ -6807,8 +8189,11 @@
         <f t="shared" si="2"/>
         <v>3.2373134328358208</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" ht="17">
+      <c r="N62">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" ht="17">
       <c r="A63" s="13">
         <v>77</v>
       </c>
@@ -6844,8 +8229,11 @@
         <f t="shared" si="2"/>
         <v>3.2238805970149254</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" ht="17">
+      <c r="N63">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" ht="17">
       <c r="A64" s="11">
         <v>78</v>
       </c>
@@ -6881,8 +8269,11 @@
         <f t="shared" si="2"/>
         <v>3.0134328358208955</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" ht="17">
+      <c r="N64">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" ht="17">
       <c r="A65" s="13">
         <v>79</v>
       </c>
@@ -6918,8 +8309,11 @@
         <f t="shared" si="2"/>
         <v>2.8223880597014928</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" ht="17">
+      <c r="N65">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" ht="17">
       <c r="A66" s="11">
         <v>80</v>
       </c>
@@ -6955,8 +8349,11 @@
         <f t="shared" si="2"/>
         <v>2.7462686567164178</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" ht="17">
+      <c r="N66">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" ht="17">
       <c r="A67" s="13">
         <v>81</v>
       </c>
@@ -6989,8 +8386,11 @@
         <v>1793000</v>
       </c>
       <c r="K67" s="8"/>
-    </row>
-    <row r="68" spans="1:11" ht="17">
+      <c r="N67">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" ht="17">
       <c r="A68" s="11">
         <v>82</v>
       </c>
@@ -7023,8 +8423,11 @@
         <v>1730000</v>
       </c>
       <c r="K68" s="8"/>
-    </row>
-    <row r="69" spans="1:11" ht="17">
+      <c r="N68">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" ht="17">
       <c r="A69" s="13">
         <v>83</v>
       </c>
@@ -7057,8 +8460,11 @@
         <v>1659000</v>
       </c>
       <c r="K69" s="8"/>
-    </row>
-    <row r="70" spans="1:11" ht="17">
+      <c r="N69">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" ht="17">
       <c r="A70" s="11">
         <v>84</v>
       </c>
@@ -7091,8 +8497,11 @@
         <v>1662000</v>
       </c>
       <c r="K70" s="8"/>
-    </row>
-    <row r="71" spans="1:11" ht="17">
+      <c r="N70">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" ht="17">
       <c r="A71" s="13">
         <v>85</v>
       </c>
@@ -7125,8 +8534,11 @@
         <v>1638000</v>
       </c>
       <c r="K71" s="8"/>
-    </row>
-    <row r="72" spans="1:11" ht="17">
+      <c r="N71">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" ht="17">
       <c r="A72" s="11">
         <v>86</v>
       </c>
@@ -7159,8 +8571,11 @@
         <v>1638000</v>
       </c>
       <c r="K72" s="8"/>
-    </row>
-    <row r="73" spans="1:11" ht="17">
+      <c r="N72">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" ht="17">
       <c r="A73" s="13">
         <v>87</v>
       </c>
@@ -7193,8 +8608,11 @@
         <v>1664000</v>
       </c>
       <c r="K73" s="8"/>
-    </row>
-    <row r="74" spans="1:11" ht="17">
+      <c r="N73">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" ht="17">
       <c r="A74" s="11">
         <v>88</v>
       </c>
@@ -7227,8 +8645,11 @@
         <v>1831000</v>
       </c>
       <c r="K74" s="8"/>
-    </row>
-    <row r="75" spans="1:11" ht="17">
+      <c r="N74">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" ht="17">
       <c r="A75" s="13">
         <v>89</v>
       </c>
@@ -7261,8 +8682,11 @@
         <v>1570000</v>
       </c>
       <c r="K75" s="8"/>
-    </row>
-    <row r="76" spans="1:11" ht="17">
+      <c r="N75">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" ht="17">
       <c r="A76" s="11">
         <v>90</v>
       </c>
@@ -7295,6 +8719,195 @@
         <v>1469000</v>
       </c>
       <c r="K76" s="8"/>
+      <c r="N76">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14">
+      <c r="N77">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14">
+      <c r="N78">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14">
+      <c r="N79">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14">
+      <c r="N80">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="81" spans="14:15">
+      <c r="N81">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="82" spans="14:15">
+      <c r="N82">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="83" spans="14:15">
+      <c r="N83">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="84" spans="14:15">
+      <c r="N84">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="85" spans="14:15">
+      <c r="N85">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="86" spans="14:15">
+      <c r="N86">
+        <v>75</v>
+      </c>
+      <c r="O86">
+        <f>173/670</f>
+        <v>0.2582089552238806</v>
+      </c>
+    </row>
+    <row r="87" spans="14:15">
+      <c r="N87">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="88" spans="14:15">
+      <c r="N88">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="89" spans="14:15">
+      <c r="N89">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="90" spans="14:15">
+      <c r="N90">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="91" spans="14:15">
+      <c r="N91">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="92" spans="14:15">
+      <c r="N92">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="93" spans="14:15">
+      <c r="N93">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="94" spans="14:15">
+      <c r="N94">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="95" spans="14:15">
+      <c r="N95">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="96" spans="14:15">
+      <c r="N96">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="97" spans="14:15">
+      <c r="N97">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="98" spans="14:15">
+      <c r="N98">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="99" spans="14:15">
+      <c r="N99">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="100" spans="14:15">
+      <c r="N100">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="101" spans="14:15">
+      <c r="N101">
+        <v>90</v>
+      </c>
+      <c r="O101">
+        <f>488/670</f>
+        <v>0.72835820895522385</v>
+      </c>
+    </row>
+    <row r="102" spans="14:15">
+      <c r="N102">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="103" spans="14:15">
+      <c r="N103">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="104" spans="14:15">
+      <c r="N104">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="105" spans="14:15">
+      <c r="N105">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="106" spans="14:15">
+      <c r="N106">
+        <v>95</v>
+      </c>
+      <c r="O106">
+        <f>783/670</f>
+        <v>1.1686567164179105</v>
+      </c>
+    </row>
+    <row r="107" spans="14:15">
+      <c r="N107">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="108" spans="14:15">
+      <c r="N108">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="109" spans="14:15">
+      <c r="N109">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="110" spans="14:15">
+      <c r="N110">
+        <v>99</v>
+      </c>
+      <c r="O110">
+        <f>1670/670</f>
+        <v>2.4925373134328357</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>